<commit_message>
Updated -1 and improved -2
Updated silkscreen on -1 and added dimm functionality for -2 as well.
</commit_message>
<xml_diff>
--- a/MR Indicator-1/MR_Indicators-1_r1_BOM.xlsx
+++ b/MR Indicator-1/MR_Indicators-1_r1_BOM.xlsx
@@ -416,21 +416,21 @@
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
+      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.48828125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="36.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="9.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="42.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="21.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="17.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="15.03"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="11.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="10.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="7.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="8.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="29.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="7.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="40.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="20.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="16.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="15.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="11.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="10.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="8.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="9.08"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="11" style="1" width="8.5"/>
   </cols>
   <sheetData>
@@ -644,7 +644,7 @@
       <c r="I8" s="6"/>
       <c r="J8" s="6"/>
     </row>
-    <row r="9" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="5" t="s">
         <v>50</v>
       </c>

</xml_diff>